<commit_message>
changes to comments foramtting
</commit_message>
<xml_diff>
--- a/sql/prosjektdagbok.xlsx
+++ b/sql/prosjektdagbok.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40169ecf656c0767/Database/prosjektoppgave-varen--22-prosjekt-30/sql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF447CA4-349E-4185-86DE-8E357210FCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{CF447CA4-349E-4185-86DE-8E357210FCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3479254-CC88-49DF-A1AE-DD511B309612}"/>
   <bookViews>
     <workbookView xWindow="5610" yWindow="3960" windowWidth="28800" windowHeight="15435" xr2:uid="{3B30E9A5-024A-4B92-8367-5AA223F9F3FA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Prosjektdagbok</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Testing av fil opplasting til db, wtforms</t>
+  </si>
+  <si>
+    <t>mulighet for sletting av comments for author og admin</t>
+  </si>
+  <si>
+    <t>mulighet for edit av content details for owner og admin</t>
   </si>
 </sst>
 </file>
@@ -438,13 +444,13 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -460,7 +466,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3">
         <f>SUM(D5:D50)</f>
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -619,10 +625,22 @@
       <c r="C20" s="1">
         <v>44670</v>
       </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>44671</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added 'likes' functionality for content and ability to sort by likes
</commit_message>
<xml_diff>
--- a/sql/prosjektdagbok.xlsx
+++ b/sql/prosjektdagbok.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40169ecf656c0767/Database/prosjektoppgave-varen--22-prosjekt-30/sql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{CF447CA4-349E-4185-86DE-8E357210FCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55EEE3D9-938A-4D60-844E-0BEB2D7369EA}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{CF447CA4-349E-4185-86DE-8E357210FCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B3C42E6-59FC-4033-B89A-9053D346D6C6}"/>
   <bookViews>
     <workbookView xWindow="5610" yWindow="3960" windowWidth="28800" windowHeight="15435" xr2:uid="{3B30E9A5-024A-4B92-8367-5AA223F9F3FA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Prosjektdagbok</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>clean up</t>
+  </si>
+  <si>
+    <t>forbedret søk og sortering. Implementert liking av innhold</t>
   </si>
 </sst>
 </file>
@@ -456,13 +459,13 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -478,7 +481,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3">
         <f>SUM(D5:D50)</f>
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -727,6 +730,12 @@
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>44681</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.25">

</xml_diff>